<commit_message>
add translations for login view
</commit_message>
<xml_diff>
--- a/src/i18n/translations.xlsx
+++ b/src/i18n/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aison/Projects/jeecg-boot-ui/src/i18n/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD7F13AA-5C94-A643-B123-79769D87E132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6547A3B4-AE81-E440-B058-A7DCF49A43E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33060" windowHeight="19560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>Keys</t>
   </si>
@@ -74,6 +74,123 @@
   </si>
   <si>
     <t>确定</t>
+  </si>
+  <si>
+    <t>login_user_placeholder</t>
+  </si>
+  <si>
+    <t>Please input the username</t>
+  </si>
+  <si>
+    <t>login_password_placeholder</t>
+  </si>
+  <si>
+    <t>Please input the password</t>
+  </si>
+  <si>
+    <t>Please input the verify code</t>
+  </si>
+  <si>
+    <t>Please input the username!</t>
+  </si>
+  <si>
+    <t>Please input the password!</t>
+  </si>
+  <si>
+    <t>请输入用户名</t>
+  </si>
+  <si>
+    <t>请输入用户名！</t>
+  </si>
+  <si>
+    <t>请输入密码</t>
+  </si>
+  <si>
+    <t>请输入密码！</t>
+  </si>
+  <si>
+    <t>请输入验证码</t>
+  </si>
+  <si>
+    <t>Please input the verify code!</t>
+  </si>
+  <si>
+    <t>请输入验证码！</t>
+  </si>
+  <si>
+    <t>Welcome</t>
+  </si>
+  <si>
+    <t>login_welcome_title</t>
+  </si>
+  <si>
+    <t>login_welcome_content</t>
+  </si>
+  <si>
+    <t>login_msg_login_error</t>
+  </si>
+  <si>
+    <t>Failed to login</t>
+  </si>
+  <si>
+    <t>login_verify_code_placeholder</t>
+  </si>
+  <si>
+    <t>login_msg_user_req</t>
+  </si>
+  <si>
+    <t>login_msg_password_req</t>
+  </si>
+  <si>
+    <t>login_msg_code_req</t>
+  </si>
+  <si>
+    <t>login_msg_code_error</t>
+  </si>
+  <si>
+    <t>您输入的验证码不正确！</t>
+  </si>
+  <si>
+    <t>欢迎</t>
+  </si>
+  <si>
+    <t>登录失败</t>
+  </si>
+  <si>
+    <t>login_msg_mobile_error</t>
+  </si>
+  <si>
+    <t>Wrong mobile number!</t>
+  </si>
+  <si>
+    <t>Wrong verify code!</t>
+  </si>
+  <si>
+    <t>您的手机号码格式不正确！</t>
+  </si>
+  <si>
+    <t>login_msg_mobile_req</t>
+  </si>
+  <si>
+    <t>Please input mobile number</t>
+  </si>
+  <si>
+    <t>login_msg_code_sending</t>
+  </si>
+  <si>
+    <t>Verify code is sending…</t>
+  </si>
+  <si>
+    <t>请输入手机号</t>
+  </si>
+  <si>
+    <t>验证码发送中…</t>
+  </si>
+  <si>
+    <t>{time}, welcome back</t>
+  </si>
+  <si>
+    <t>{time}，欢迎回来</t>
   </si>
 </sst>
 </file>
@@ -130,10 +247,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="206" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D6"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -485,7 +601,7 @@
     <col min="3" max="3" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -496,51 +612,51 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>7</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -550,12 +666,154 @@
       <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" t="s">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="C1 B1" numberStoredAsText="1"/>
+    <ignoredError sqref="C1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>